<commit_message>
Juno: check in to OLPRODLOC.
</commit_message>
<xml_diff>
--- a/ResourceFiles/Contoso Chai Tea market trends 2023.xlsx
+++ b/ResourceFiles/Contoso Chai Tea market trends 2023.xlsx
@@ -52,56 +52,61 @@
   <si>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Gesamt-Sales Chai (Einheiten)</t>
+      <t>Chai-Gesamtumsatz (Einheiten)</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Sales selbstgemachter Chai (Einheiten)</t>
+      <t>Artisanal Chai-Umsatz (Einheiten)</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Sales fertiger Chai (Einheiten)</t>
+      <t>Vorgefertigter Chai-Umsatz (Einheiten)</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Social-Media-Engagement (Aufrufe)</t>
+      <t>Social-Media-Interaktion (Ansichten)</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Online-Suchanfragen für Chai</t>
+      <t>Onlinesuchen nach Chai</t>
     </r>
   </si>
   <si>
@@ -123,7 +128,7 @@
   <numFmts count="1">
     <numFmt numFmtId="177" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,12 +152,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -434,11 +433,11 @@
   <autoFilter ref="A1:F14"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Datum" dataDxfId="0"/>
-    <tableColumn id="2" name="Gesamt-Sales Chai (Einheiten)"/>
-    <tableColumn id="3" name="Sales selbstgemachter Chai (Einheiten)"/>
-    <tableColumn id="4" name="Sales fertiger Chai (Einheiten)"/>
-    <tableColumn id="5" name="Social-Media-Engagement (Aufrufe)"/>
-    <tableColumn id="6" name="Online-Suchanfragen für Chai"/>
+    <tableColumn id="2" name="Chai-Gesamtumsatz (Einheiten)"/>
+    <tableColumn id="3" name="Artisanal Chai-Umsatz (Einheiten)"/>
+    <tableColumn id="4" name="Vorgefertigter Chai-Umsatz (Einheiten)"/>
+    <tableColumn id="5" name="Social-Media-Interaktion (Ansichten)"/>
+    <tableColumn id="6" name="Onlinesuchen nach Chai"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>

<commit_message>
Copy Files From Source Repo (2024-07-19 18:34)
</commit_message>
<xml_diff>
--- a/ResourceFiles/Contoso Chai Tea market trends 2023.xlsx
+++ b/ResourceFiles/Contoso Chai Tea market trends 2023.xlsx
@@ -52,56 +52,61 @@
   <si>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Gesamt-Sales Chai (Einheiten)</t>
+      <t>Chai-Gesamtumsatz (Einheiten)</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Sales selbstgemachter Chai (Einheiten)</t>
+      <t>Artisanal Chai-Umsatz (Einheiten)</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Sales fertiger Chai (Einheiten)</t>
+      <t>Vorgefertigter Chai-Umsatz (Einheiten)</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Social-Media-Engagement (Aufrufe)</t>
+      <t>Social-Media-Interaktion (Ansichten)</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Online-Suchanfragen für Chai</t>
+      <t>Onlinesuchen nach Chai</t>
     </r>
   </si>
   <si>
@@ -123,7 +128,7 @@
   <numFmts count="1">
     <numFmt numFmtId="177" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,12 +152,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -434,11 +433,11 @@
   <autoFilter ref="A1:F14"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Datum" dataDxfId="0"/>
-    <tableColumn id="2" name="Gesamt-Sales Chai (Einheiten)"/>
-    <tableColumn id="3" name="Sales selbstgemachter Chai (Einheiten)"/>
-    <tableColumn id="4" name="Sales fertiger Chai (Einheiten)"/>
-    <tableColumn id="5" name="Social-Media-Engagement (Aufrufe)"/>
-    <tableColumn id="6" name="Online-Suchanfragen für Chai"/>
+    <tableColumn id="2" name="Chai-Gesamtumsatz (Einheiten)"/>
+    <tableColumn id="3" name="Artisanal Chai-Umsatz (Einheiten)"/>
+    <tableColumn id="4" name="Vorgefertigter Chai-Umsatz (Einheiten)"/>
+    <tableColumn id="5" name="Social-Media-Interaktion (Ansichten)"/>
+    <tableColumn id="6" name="Onlinesuchen nach Chai"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>

<commit_message>
Copy Files From Source Repo (2025-02-10 19:17)
</commit_message>
<xml_diff>
--- a/ResourceFiles/Contoso Chai Tea market trends 2023.xlsx
+++ b/ResourceFiles/Contoso Chai Tea market trends 2023.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <r>
       <rPr>
@@ -46,7 +46,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Datum</t>
+      <t>Date</t>
     </r>
   </si>
   <si>
@@ -58,7 +58,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Chai-Gesamtumsatz (Einheiten)</t>
+      <t>Chai-Verkäufe insgesamt (Einheiten)</t>
     </r>
   </si>
   <si>
@@ -118,6 +118,28 @@
         <family val="2"/>
       </rPr>
       <t>–4 %</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>4:36</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>17:05</t>
     </r>
   </si>
 </sst>
@@ -432,8 +454,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F14" totalsRowShown="0" headerRowDxfId="3" tableBorderDxfId="1" headerRowBorderDxfId="2">
   <autoFilter ref="A1:F14"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Datum" dataDxfId="0"/>
-    <tableColumn id="2" name="Chai-Gesamtumsatz (Einheiten)"/>
+    <tableColumn id="1" name="Date" dataDxfId="0"/>
+    <tableColumn id="2" name="Chai-Verkäufe insgesamt (Einheiten)"/>
     <tableColumn id="3" name="Artisanal Chai-Umsatz (Einheiten)"/>
     <tableColumn id="4" name="Vorgefertigter Chai-Umsatz (Einheiten)"/>
     <tableColumn id="5" name="Social-Media-Interaktion (Ansichten)"/>
@@ -861,11 +883,11 @@
       <c r="C6">
         <v>499</v>
       </c>
-      <c r="D6">
-        <v>436</v>
-      </c>
-      <c r="E6">
-        <v>1705</v>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
       </c>
       <c r="F6">
         <v>2996</v>

</xml_diff>